<commit_message>
Update clean code GetInfoRollbackBTransactionHasIncomingEntry and RollbackBTransactionHasIncomingEntry Fix bug ExportBBC
</commit_message>
<xml_diff>
--- a/aspnet-core/src/FinanceManagement.Web.Host/wwwroot/Template_BaoCaoChi.xlsx
+++ b/aspnet-core/src/FinanceManagement.Web.Host/wwwroot/Template_BaoCaoChi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\NCC\Trainning_NET\Finfast\Finfast_git_dev\ncc-erp-finance\aspnet-core\src\FinanceManagement.Web.Host\wwwroot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E893059-EBAA-4D15-AB04-4F952F56BA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD333616-6319-43BD-97F5-722A2568E21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{937F6B67-9F17-4F48-8DB3-5C3750E8288D}"/>
   </bookViews>
@@ -153,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -170,8 +170,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -489,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D813843F-F088-4930-A3C0-D2FB9D8B7699}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J1" activeCellId="1" sqref="G1:G1048576 J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -500,11 +518,11 @@
     <col min="3" max="3" width="23" style="2" customWidth="1"/>
     <col min="4" max="4" width="39.5546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="41.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="27.44140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="27.44140625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" style="10" customWidth="1"/>
     <col min="8" max="8" width="15.88671875" style="2" customWidth="1"/>
     <col min="9" max="9" width="19.109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="35.33203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="35.33203125" style="10" customWidth="1"/>
     <col min="11" max="11" width="32" style="2" customWidth="1"/>
     <col min="12" max="12" width="30.44140625" style="2" customWidth="1"/>
   </cols>
@@ -513,15 +531,15 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="3" t="s">
@@ -539,10 +557,10 @@
       <c r="E5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="11" t="s">
         <v>7</v>
       </c>
       <c r="H5" s="4" t="s">
@@ -551,7 +569,7 @@
       <c r="I5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="11" t="s">
         <v>10</v>
       </c>
       <c r="K5" s="3" t="s">
@@ -567,11 +585,11 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="12"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
+      <c r="J6" s="12"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>

</xml_diff>